<commit_message>
Integrate LaTeX in text attribute: test cases
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>uid</t>
   </si>
@@ -97,6 +97,13 @@
   </si>
   <si>
     <t>REQ2-001</t>
+  </si>
+  <si>
+    <t>Hello, world!
+Test Math Expressions in Latex Style:
+Inline Style 1: $a \ne 0$
+Inline Style 2: \(ax^2 + bx + c = 0\)
+Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
   </si>
 </sst>
 </file>
@@ -465,162 +472,162 @@
     <col customWidth="1" max="9" min="9" width="35.5"/>
   </cols>
   <sheetData>
-    <row spans="1:9" r="1">
-      <c t="s" s="1" r="A1">
+    <row r="1" spans="1:9">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c t="s" s="1" r="B1">
-        <v>1</v>
-      </c>
-      <c t="s" s="1" r="C1">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c t="s" s="1" r="D1">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c t="s" s="1" r="E1">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c t="s" s="1" r="F1">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c t="s" s="1" r="G1">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c t="s" s="1" r="H1">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c t="s" s="1" r="I1">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row spans="1:9" r="2">
-      <c t="s" s="2" r="A2">
+    <row r="2" spans="1:9">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="s" s="2" r="B2">
+      <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c t="s" s="2" r="C2">
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
-      <c t="s" s="2" r="D2"/>
-      <c t="s" s="2" r="E2">
+      <c r="D2" s="2" t="s"/>
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c t="b" s="2" r="F2">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G2">
+      <c r="F2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H2">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I2"/>
+      <c r="H2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s"/>
     </row>
-    <row spans="1:9" r="3">
-      <c t="s" s="2" r="A3">
+    <row r="3" spans="1:9">
+      <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
-      <c t="s" s="2" r="B3">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c t="s" s="2" r="C3">
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c t="s" s="2" r="D3">
+      <c r="D3" s="2" t="s">
         <v>16</v>
       </c>
-      <c t="s" s="2" r="E3">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="b" s="2" r="F3">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G3">
+      <c r="F3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H3">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I3"/>
+      <c r="H3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" s="2" t="s"/>
     </row>
-    <row spans="1:9" r="4">
-      <c t="s" s="2" r="A4">
+    <row r="4" spans="1:9">
+      <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
-      <c t="s" s="2" r="B4">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c t="s" s="2" r="C4">
+      <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="2" r="D4"/>
-      <c t="s" s="2" r="E4"/>
-      <c t="b" s="2" r="F4">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G4">
+      <c r="D4" s="2" t="s"/>
+      <c r="E4" s="2" t="s"/>
+      <c r="F4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H4">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I4"/>
+      <c r="H4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2" t="s"/>
     </row>
-    <row spans="1:9" r="5">
-      <c t="s" s="2" r="A5">
+    <row r="5" spans="1:9">
+      <c r="A5" s="2" t="s">
         <v>20</v>
       </c>
-      <c t="s" s="2" r="B5">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="2" r="C5">
+      <c r="C5" s="2" t="s">
         <v>19</v>
       </c>
-      <c t="s" s="2" r="D5"/>
-      <c t="s" s="2" r="E5"/>
-      <c t="b" s="2" r="F5">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G5">
+      <c r="D5" s="2" t="s"/>
+      <c r="E5" s="2" t="s"/>
+      <c r="F5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H5">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I5">
+      <c r="H5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row spans="1:9" r="6">
-      <c t="s" s="2" r="A6">
+    <row r="6" spans="1:9">
+      <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c t="s" s="2" r="B6">
+      <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
-      <c t="s" s="2" r="C6">
-        <v>19</v>
-      </c>
-      <c t="s" s="2" r="D6"/>
-      <c t="s" s="2" r="E6">
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s"/>
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c t="b" s="2" r="F6">
-        <v>1</v>
-      </c>
-      <c t="b" s="2" r="G6">
+      <c r="F6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c t="b" s="2" r="H6">
-        <v>1</v>
-      </c>
-      <c t="s" s="2" r="I6"/>
+      <c r="H6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" s="2" t="s"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I1"/>
-  <pageMargins footer="0.5" top="1" bottom="1" left="0.75" header="0.5" right="0.75"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integrate plantuml-markdown extension for item text attribute: exemplary test case
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
   <si>
     <t>uid</t>
   </si>
@@ -93,7 +93,27 @@
     <t>2.1</t>
   </si>
   <si>
-    <t>b5fbcc355112791bbcd2ea881c7c5f81</t>
+    <t>Hello, world!
+```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
+@startuml
+Author --&gt; (Create Document)
+Author --&gt; (Create Item)
+Author --&gt; (Link Item to Document)
+Author --&gt; (Link Item to other Item)
+Author --&gt; (Edit Item)
+Author --&gt; (Review Item)
+Author -&gt; (Delete Item)
+Author -&gt; (Delete Document)
+(Export) &lt;- (Author)
+(Import) &lt;- (Author)
+Reviewer --&gt; (Review Item)
+System --&gt; (Suspect Changes)
+System --&gt; (Integrity)
+@enduml
+```</t>
+  </si>
+  <si>
+    <t>50ae164a198e612dee696cc80942dc29</t>
   </si>
   <si>
     <t>REQ2-001</t>
@@ -584,7 +604,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D5" s="2" t="s"/>
       <c r="E5" s="2" t="s"/>
@@ -598,18 +618,18 @@
         <v>1</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2" t="s"/>
       <c r="E6" s="2" t="s">

</xml_diff>

<commit_message>
WIP: RFC: Item#ref: initial support of many ref items
This change enables the ref field to support references to multiple files
instead of a single file reference which was old behavior.

The attempt is made to preserve the existing behavior as much as possible on
both Item model and GUI levels.

[skip ci]
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -1,137 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames>
-    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</s:definedName>
-  </s:definedNames>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
-  <si>
-    <t>uid</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>links</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>derived</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>normative</t>
-  </si>
-  <si>
-    <t>reviewed</t>
-  </si>
-  <si>
-    <t>REQ001</t>
-  </si>
-  <si>
-    <t>1.2.3</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
-tempor incididunt ut labore et dolore magna aliqua.
-Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
-aliquip ex ea commodo consequat.
-Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
-eu fugiat nulla pariatur.
-Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
-deserunt mollit anim id est laborum.</t>
-  </si>
-  <si>
-    <t>SYS001
-SYS002:abc123</t>
-  </si>
-  <si>
-    <t>REQ003</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>Unicode: -40° ±1%</t>
-  </si>
-  <si>
-    <t>REF123</t>
-  </si>
-  <si>
-    <t>REQ004</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>Hello, world!</t>
-  </si>
-  <si>
-    <t>REQ002</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>Hello, world!
-```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
-@startuml
-Author --&gt; (Create Document)
-Author --&gt; (Create Item)
-Author --&gt; (Link Item to Document)
-Author --&gt; (Link Item to other Item)
-Author --&gt; (Edit Item)
-Author --&gt; (Review Item)
-Author -&gt; (Delete Item)
-Author -&gt; (Delete Document)
-(Export) &lt;- (Author)
-(Import) &lt;- (Author)
-Reviewer --&gt; (Review Item)
-System --&gt; (Suspect Changes)
-System --&gt; (Integrity)
-@enduml
-```</t>
-  </si>
-  <si>
-    <t>Plantuml</t>
-  </si>
-  <si>
-    <t>50ae164a198e612dee696cc80942dc29</t>
-  </si>
-  <si>
-    <t>REQ2-001</t>
-  </si>
-  <si>
-    <t>Hello, world!
-Test Math Expressions in Latex Style:
-Inline Style 1: $a \ne 0$
-Inline Style 2: \(ax^2 + bx + c = 0\)
-Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
-  </si>
-</sst>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</definedName>
+  </definedNames>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -139,23 +21,19 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="00000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -174,18 +52,17 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -474,24 +351,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
       <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="11.5"/>
     <col customWidth="1" max="2" min="2" width="8.5"/>
     <col customWidth="1" max="3" min="3" width="65"/>
-    <col customWidth="1" max="4" min="4" width="9.5"/>
-    <col customWidth="1" max="5" min="5" width="16.5"/>
+    <col customWidth="1" max="4" min="4" width="36.5"/>
+    <col customWidth="1" max="5" min="5" width="42.5"/>
     <col customWidth="1" max="6" min="6" width="9.5"/>
     <col customWidth="1" max="7" min="7" width="10.5"/>
     <col customWidth="1" max="8" min="8" width="11.5"/>
@@ -499,51 +377,87 @@
     <col customWidth="1" max="10" min="10" width="35.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>uid</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>links</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>derived</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>header</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>normative</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>reviewed</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s"/>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>1.2.3</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
+tempor incididunt ut labore et dolore magna aliqua.
+Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
+aliquip ex ea commodo consequat.
+Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
+eu fugiat nulla pariatur.
+Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
+deserunt mollit anim id est laborum.</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>SYS001
+SYS002:abc123</t>
+        </is>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>
@@ -551,27 +465,37 @@
       <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s"/>
+      <c r="H2" s="2" t="inlineStr"/>
       <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="2" t="s"/>
+      <c r="J2" s="2" t="inlineStr"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>REQ003</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>1.4</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Unicode: -40° ±1%</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>REF123</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
       </c>
       <c r="F3" s="2" t="b">
         <v>1</v>
@@ -579,92 +503,180 @@
       <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s"/>
+      <c r="H3" s="2" t="inlineStr"/>
       <c r="I3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s"/>
+      <c r="J3" s="2" t="inlineStr"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s"/>
-      <c r="E4" s="2" t="s"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>REQ006</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>1.5</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>type:file,path:external/text.txt
+type:file,path:external/text2.txt</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>REQ001:35ed54323e3054c33ae5545fffdbbbf5</t>
+        </is>
+      </c>
       <c r="F4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s"/>
+      <c r="H4" s="2" t="inlineStr"/>
       <c r="I4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="2" t="s"/>
+      <c r="J4" s="2" t="inlineStr">
+        <is>
+          <t>c442316131ca0225595ae257f3b4583d</t>
+        </is>
+      </c>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s"/>
-      <c r="E5" s="2" t="s"/>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>REQ004</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr"/>
       <c r="F5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="H5" s="2" t="inlineStr"/>
       <c r="I5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="J5" s="2" t="inlineStr"/>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s"/>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>REQ002</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!
+```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
+@startuml
+Author --&gt; (Create Document)
+Author --&gt; (Create Item)
+Author --&gt; (Link Item to Document)
+Author --&gt; (Link Item to other Item)
+Author --&gt; (Edit Item)
+Author --&gt; (Review Item)
+Author -&gt; (Delete Item)
+Author -&gt; (Delete Document)
+(Export) &lt;- (Author)
+(Import) &lt;- (Author)
+Reviewer --&gt; (Review Item)
+System --&gt; (Suspect Changes)
+System --&gt; (Integrity)
+@enduml
+```</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr"/>
       <c r="F6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="s"/>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>Plantuml</t>
+        </is>
+      </c>
       <c r="I6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="2" t="s"/>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>50ae164a198e612dee696cc80942dc29</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>REQ2-001</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!
+Test Math Expressions in Latex Style:
+Inline Style 1: $a \ne 0$
+Inline Style 2: \(ax^2 + bx + c = 0\)
+Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr"/>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="inlineStr"/>
+      <c r="I7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update export.xlsx with header column
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -10,14 +10,14 @@
     <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </s:sheets>
   <s:definedNames>
-    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$I$1</s:definedName>
+    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</s:definedName>
   </s:definedNames>
   <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
 </s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
     <t>uid</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>derived</t>
+  </si>
+  <si>
+    <t>header</t>
   </si>
   <si>
     <t>normative</t>
@@ -111,6 +114,9 @@
 System --&gt; (Integrity)
 @enduml
 ```</t>
+  </si>
+  <si>
+    <t>Plantuml</t>
   </si>
   <si>
     <t>50ae164a198e612dee696cc80942dc29</t>
@@ -472,7 +478,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -488,11 +494,12 @@
     <col customWidth="1" max="5" min="5" width="16.5"/>
     <col customWidth="1" max="6" min="6" width="9.5"/>
     <col customWidth="1" max="7" min="7" width="10.5"/>
-    <col customWidth="1" max="8" min="8" width="12.5"/>
-    <col customWidth="1" max="9" min="9" width="35.5"/>
+    <col customWidth="1" max="8" min="8" width="11.5"/>
+    <col customWidth="1" max="9" min="9" width="12.5"/>
+    <col customWidth="1" max="10" min="10" width="35.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,20 +527,23 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s"/>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>
@@ -541,26 +551,27 @@
       <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s"/>
+      <c r="H2" s="2" t="s"/>
+      <c r="I2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2" t="s"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="b">
         <v>1</v>
@@ -568,20 +579,21 @@
       <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="s"/>
+      <c r="H3" s="2" t="s"/>
+      <c r="I3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s"/>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s"/>
       <c r="E4" s="2" t="s"/>
@@ -591,20 +603,21 @@
       <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s"/>
+      <c r="H4" s="2" t="s"/>
+      <c r="I4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s"/>
       <c r="E5" s="2" t="s"/>
@@ -614,26 +627,29 @@
       <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>23</v>
+      <c r="H5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2" t="s"/>
       <c r="E6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="b">
         <v>1</v>
@@ -641,13 +657,14 @@
       <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="s"/>
+      <c r="H6" s="2" t="s"/>
+      <c r="I6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2" t="s"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:J1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RFC: Item#references: initial support of many ref items (Take 2)
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -369,12 +369,13 @@
     <col customWidth="1" max="2" min="2" width="8.5"/>
     <col customWidth="1" max="3" min="3" width="65"/>
     <col customWidth="1" max="4" min="4" width="9.5"/>
-    <col customWidth="1" max="5" min="5" width="16.5"/>
-    <col customWidth="1" max="6" min="6" width="9.5"/>
-    <col customWidth="1" max="7" min="7" width="10.5"/>
-    <col customWidth="1" max="8" min="8" width="11.5"/>
-    <col customWidth="1" max="9" min="9" width="12.5"/>
-    <col customWidth="1" max="10" min="10" width="35.5"/>
+    <col customWidth="1" max="5" min="5" width="36.5"/>
+    <col customWidth="1" max="6" min="6" width="42.5"/>
+    <col customWidth="1" max="7" min="7" width="9.5"/>
+    <col customWidth="1" max="8" min="8" width="10.5"/>
+    <col customWidth="1" max="9" min="9" width="11.5"/>
+    <col customWidth="1" max="10" min="10" width="12.5"/>
+    <col customWidth="1" max="11" min="11" width="35.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -400,30 +401,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>links</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>active</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>derived</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>header</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>normative</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>reviewed</t>
         </is>
@@ -453,23 +459,24 @@
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr"/>
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>SYS001
 SYS002:abc123</t>
         </is>
       </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
       <c r="G2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="inlineStr"/>
-      <c r="I2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="inlineStr"/>
+      <c r="I2" s="2" t="inlineStr"/>
+      <c r="J2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -492,32 +499,33 @@
           <t>REF123</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr"/>
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>REQ001</t>
         </is>
       </c>
-      <c r="F3" s="2" t="b">
-        <v>1</v>
-      </c>
       <c r="G3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="inlineStr"/>
-      <c r="I3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2" t="inlineStr"/>
+      <c r="I3" s="2" t="inlineStr"/>
+      <c r="J3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>REQ004</t>
+          <t>REQ006</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -526,31 +534,76 @@
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr"/>
-      <c r="E4" s="2" t="inlineStr"/>
-      <c r="F4" s="2" t="b">
-        <v>1</v>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>type:file,path:external/text.txt
+type:file,path:external/text2.txt</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>REQ001:35ed54323e3054c33ae5545fffdbbbf5</t>
+        </is>
       </c>
       <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="inlineStr"/>
-      <c r="I4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2" t="inlineStr"/>
+      <c r="I4" s="2" t="inlineStr"/>
+      <c r="J4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>c442316131ca0225595ae257f3b4583d</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
+          <t>REQ004</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr"/>
+      <c r="F5" s="2" t="inlineStr"/>
+      <c r="G5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="inlineStr"/>
+      <c r="J5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
           <t>REQ002</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>2.1</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>Hello, world!
 ```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
@@ -572,40 +625,41 @@
 ```</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr"/>
-      <c r="E5" s="2" t="inlineStr"/>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="b">
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr"/>
+      <c r="F6" s="2" t="inlineStr"/>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="inlineStr">
+      <c r="I6" s="2" t="inlineStr">
         <is>
           <t>Plantuml</t>
         </is>
       </c>
-      <c r="I5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2" t="inlineStr">
+      <c r="J6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
         <is>
           <t>50ae164a198e612dee696cc80942dc29</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>REQ2-001</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>2.1</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Hello, world!
 Test Math Expressions in Latex Style:
@@ -614,26 +668,27 @@
 Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr"/>
-      <c r="E6" s="2" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr"/>
+      <c r="E7" s="2" t="inlineStr"/>
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>REQ001</t>
         </is>
       </c>
-      <c r="F6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2" t="b">
+      <c r="G7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="inlineStr"/>
-      <c r="I6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2" t="inlineStr"/>
+      <c r="I7" s="2" t="inlineStr"/>
+      <c r="J7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A1:K1"/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RFC: Item#references: initial support of many ref items (Take 3)
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -356,7 +356,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
@@ -369,12 +369,13 @@
     <col customWidth="1" max="2" min="2" width="8.5"/>
     <col customWidth="1" max="3" min="3" width="65"/>
     <col customWidth="1" max="4" min="4" width="9.5"/>
-    <col customWidth="1" max="5" min="5" width="16.5"/>
-    <col customWidth="1" max="6" min="6" width="9.5"/>
-    <col customWidth="1" max="7" min="7" width="10.5"/>
-    <col customWidth="1" max="8" min="8" width="11.5"/>
-    <col customWidth="1" max="9" min="9" width="12.5"/>
-    <col customWidth="1" max="10" min="10" width="47.5"/>
+    <col customWidth="1" max="5" min="5" width="50.5"/>
+    <col customWidth="1" max="6" min="6" width="42.5"/>
+    <col customWidth="1" max="7" min="7" width="9.5"/>
+    <col customWidth="1" max="8" min="8" width="10.5"/>
+    <col customWidth="1" max="9" min="9" width="11.5"/>
+    <col customWidth="1" max="10" min="10" width="12.5"/>
+    <col customWidth="1" max="11" min="11" width="47.5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -400,30 +401,35 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>references</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>links</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>active</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>derived</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>header</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>normative</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>reviewed</t>
         </is>
@@ -453,23 +459,24 @@
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr"/>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr"/>
+      <c r="F2" s="2" t="inlineStr">
         <is>
           <t>SYS001
 SYS002:abc123</t>
         </is>
       </c>
-      <c r="F2" s="2" t="b">
-        <v>1</v>
-      </c>
       <c r="G2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="inlineStr"/>
-      <c r="I2" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2" t="inlineStr"/>
+      <c r="I2" s="2" t="inlineStr"/>
+      <c r="J2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -492,32 +499,33 @@
           <t>REF123</t>
         </is>
       </c>
-      <c r="E3" s="2" t="inlineStr">
+      <c r="E3" s="2" t="inlineStr"/>
+      <c r="F3" s="2" t="inlineStr">
         <is>
           <t>REQ001</t>
         </is>
       </c>
-      <c r="F3" s="2" t="b">
-        <v>1</v>
-      </c>
       <c r="G3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="inlineStr"/>
-      <c r="I3" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2" t="inlineStr"/>
+      <c r="I3" s="2" t="inlineStr"/>
+      <c r="J3" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="2" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>REQ004</t>
+          <t>REQ006</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>1.6</t>
+          <t>1.5</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
@@ -526,31 +534,76 @@
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr"/>
-      <c r="E4" s="2" t="inlineStr"/>
-      <c r="F4" s="2" t="b">
-        <v>1</v>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>type:file,path:external/text.txt,keyword:REF123
+type:file,path:external/text2.txt</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>REQ001:35ed54323e3054c33ae5545fffdbbbf5</t>
+        </is>
       </c>
       <c r="G4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="inlineStr"/>
-      <c r="I4" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2" t="inlineStr"/>
+      <c r="I4" s="2" t="inlineStr"/>
+      <c r="J4" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2" t="inlineStr">
+        <is>
+          <t>c442316131ca0225595ae257f3b4583d</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
+          <t>REQ004</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr"/>
+      <c r="F5" s="2" t="inlineStr"/>
+      <c r="G5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2" t="inlineStr"/>
+      <c r="J5" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="2" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
           <t>REQ002</t>
         </is>
       </c>
-      <c r="B5" s="2" t="inlineStr">
+      <c r="B6" s="2" t="inlineStr">
         <is>
           <t>2.1</t>
         </is>
       </c>
-      <c r="C5" s="2" t="inlineStr">
+      <c r="C6" s="2" t="inlineStr">
         <is>
           <t>Hello, world!
 ```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
@@ -572,40 +625,41 @@
 ```</t>
         </is>
       </c>
-      <c r="D5" s="2" t="inlineStr"/>
-      <c r="E5" s="2" t="inlineStr"/>
-      <c r="F5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2" t="b">
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr"/>
+      <c r="F6" s="2" t="inlineStr"/>
+      <c r="G6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="inlineStr">
+      <c r="I6" s="2" t="inlineStr">
         <is>
           <t>Plantuml</t>
         </is>
       </c>
-      <c r="I5" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2" t="inlineStr">
+      <c r="J6" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
         <is>
           <t>1PvBLmy0xmdK_zLKrLu1au0wlIw_zsD6A8Oc5F4zWxU=</t>
         </is>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>REQ2-001</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>2.1</t>
         </is>
       </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="C7" s="2" t="inlineStr">
         <is>
           <t>Hello, world!
 Test Math Expressions in Latex Style:
@@ -614,26 +668,27 @@
 Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
         </is>
       </c>
-      <c r="D6" s="2" t="inlineStr"/>
-      <c r="E6" s="2" t="inlineStr">
+      <c r="D7" s="2" t="inlineStr"/>
+      <c r="E7" s="2" t="inlineStr"/>
+      <c r="F7" s="2" t="inlineStr">
         <is>
           <t>REQ001</t>
         </is>
       </c>
-      <c r="F6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2" t="b">
+      <c r="G7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="inlineStr"/>
-      <c r="I6" s="2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2" t="inlineStr"/>
+      <c r="I7" s="2" t="inlineStr"/>
+      <c r="J7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="inlineStr"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A1:K1"/>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Switch to SHA1 for detecting changes to files
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -1,137 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames>
-    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</s:definedName>
-  </s:definedNames>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
-  <si>
-    <t>uid</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>links</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>derived</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>normative</t>
-  </si>
-  <si>
-    <t>reviewed</t>
-  </si>
-  <si>
-    <t>REQ001</t>
-  </si>
-  <si>
-    <t>1.2.3</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
-tempor incididunt ut labore et dolore magna aliqua.
-Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
-aliquip ex ea commodo consequat.
-Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
-eu fugiat nulla pariatur.
-Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
-deserunt mollit anim id est laborum.</t>
-  </si>
-  <si>
-    <t>SYS001
-SYS002:abc123</t>
-  </si>
-  <si>
-    <t>REQ003</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>Unicode: -40° ±1%</t>
-  </si>
-  <si>
-    <t>REF123</t>
-  </si>
-  <si>
-    <t>REQ004</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>Hello, world!</t>
-  </si>
-  <si>
-    <t>REQ002</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>Hello, world!
-```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
-@startuml
-Author --&gt; (Create Document)
-Author --&gt; (Create Item)
-Author --&gt; (Link Item to Document)
-Author --&gt; (Link Item to other Item)
-Author --&gt; (Edit Item)
-Author --&gt; (Review Item)
-Author -&gt; (Delete Item)
-Author -&gt; (Delete Document)
-(Export) &lt;- (Author)
-(Import) &lt;- (Author)
-Reviewer --&gt; (Review Item)
-System --&gt; (Suspect Changes)
-System --&gt; (Integrity)
-@enduml
-```</t>
-  </si>
-  <si>
-    <t>Plantuml</t>
-  </si>
-  <si>
-    <t>50ae164a198e612dee696cc80942dc29</t>
-  </si>
-  <si>
-    <t>REQ2-001</t>
-  </si>
-  <si>
-    <t>Hello, world!
-Test Math Expressions in Latex Style:
-Inline Style 1: $a \ne 0$
-Inline Style 2: \(ax^2 + bx + c = 0\)
-Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
-  </si>
-</sst>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</definedName>
+  </definedNames>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -139,23 +21,19 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="00000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -174,18 +52,17 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -474,9 +351,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -485,7 +363,7 @@
       <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="11.5"/>
     <col customWidth="1" max="2" min="2" width="8.5"/>
@@ -496,54 +374,90 @@
     <col customWidth="1" max="7" min="7" width="10.5"/>
     <col customWidth="1" max="8" min="8" width="11.5"/>
     <col customWidth="1" max="9" min="9" width="12.5"/>
-    <col customWidth="1" max="10" min="10" width="35.5"/>
+    <col customWidth="1" max="10" min="10" width="43.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>uid</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>links</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>derived</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>header</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>normative</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>reviewed</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s"/>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>1.2.3</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
+tempor incididunt ut labore et dolore magna aliqua.
+Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
+aliquip ex ea commodo consequat.
+Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
+eu fugiat nulla pariatur.
+Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
+deserunt mollit anim id est laborum.</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>SYS001
+SYS002:abc123</t>
+        </is>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>
@@ -551,27 +465,37 @@
       <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s"/>
+      <c r="H2" s="2" t="inlineStr"/>
       <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="2" t="s"/>
+      <c r="J2" s="2" t="inlineStr"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>REQ003</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>1.4</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Unicode: -40° ±1%</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>REF123</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
       </c>
       <c r="F3" s="2" t="b">
         <v>1</v>
@@ -579,77 +503,122 @@
       <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s"/>
+      <c r="H3" s="2" t="inlineStr"/>
       <c r="I3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s"/>
+      <c r="J3" s="2" t="inlineStr"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s"/>
-      <c r="E4" s="2" t="s"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>REQ004</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr"/>
+      <c r="E4" s="2" t="inlineStr"/>
       <c r="F4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s"/>
+      <c r="H4" s="2" t="inlineStr"/>
       <c r="I4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="2" t="s"/>
+      <c r="J4" s="2" t="inlineStr"/>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s"/>
-      <c r="E5" s="2" t="s"/>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>REQ002</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!
+```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
+@startuml
+Author --&gt; (Create Document)
+Author --&gt; (Create Item)
+Author --&gt; (Link Item to Document)
+Author --&gt; (Link Item to other Item)
+Author --&gt; (Edit Item)
+Author --&gt; (Review Item)
+Author -&gt; (Delete Item)
+Author -&gt; (Delete Document)
+(Export) &lt;- (Author)
+(Import) &lt;- (Author)
+Reviewer --&gt; (Review Item)
+System --&gt; (Suspect Changes)
+System --&gt; (Integrity)
+@enduml
+```</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr"/>
       <c r="F5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>Plantuml</t>
+        </is>
       </c>
       <c r="I5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>7186a9a1fd2d84d5c92ebcbaf6d3291f32f998ee</t>
+        </is>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s"/>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>REQ2-001</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!
+Test Math Expressions in Latex Style:
+Inline Style 1: $a \ne 0$
+Inline Style 2: \(ax^2 + bx + c = 0\)
+Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
       </c>
       <c r="F6" s="2" t="b">
         <v>1</v>
@@ -657,14 +626,14 @@
       <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="s"/>
+      <c r="H6" s="2" t="inlineStr"/>
       <c r="I6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="2" t="s"/>
+      <c r="J6" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Switch to SHA256 for detecting changes to files
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -1,137 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames>
-    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</s:definedName>
-  </s:definedNames>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
-  <si>
-    <t>uid</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>links</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>derived</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>normative</t>
-  </si>
-  <si>
-    <t>reviewed</t>
-  </si>
-  <si>
-    <t>REQ001</t>
-  </si>
-  <si>
-    <t>1.2.3</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
-tempor incididunt ut labore et dolore magna aliqua.
-Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
-aliquip ex ea commodo consequat.
-Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
-eu fugiat nulla pariatur.
-Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
-deserunt mollit anim id est laborum.</t>
-  </si>
-  <si>
-    <t>SYS001
-SYS002:abc123</t>
-  </si>
-  <si>
-    <t>REQ003</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>Unicode: -40° ±1%</t>
-  </si>
-  <si>
-    <t>REF123</t>
-  </si>
-  <si>
-    <t>REQ004</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>Hello, world!</t>
-  </si>
-  <si>
-    <t>REQ002</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>Hello, world!
-```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
-@startuml
-Author --&gt; (Create Document)
-Author --&gt; (Create Item)
-Author --&gt; (Link Item to Document)
-Author --&gt; (Link Item to other Item)
-Author --&gt; (Edit Item)
-Author --&gt; (Review Item)
-Author -&gt; (Delete Item)
-Author -&gt; (Delete Document)
-(Export) &lt;- (Author)
-(Import) &lt;- (Author)
-Reviewer --&gt; (Review Item)
-System --&gt; (Suspect Changes)
-System --&gt; (Integrity)
-@enduml
-```</t>
-  </si>
-  <si>
-    <t>Plantuml</t>
-  </si>
-  <si>
-    <t>50ae164a198e612dee696cc80942dc29</t>
-  </si>
-  <si>
-    <t>REQ2-001</t>
-  </si>
-  <si>
-    <t>Hello, world!
-Test Math Expressions in Latex Style:
-Inline Style 1: $a \ne 0$
-Inline Style 2: \(ax^2 + bx + c = 0\)
-Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
-  </si>
-</sst>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</definedName>
+  </definedNames>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -139,23 +21,19 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="00000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -174,18 +52,17 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -474,9 +351,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -485,7 +363,7 @@
       <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="11.5"/>
     <col customWidth="1" max="2" min="2" width="8.5"/>
@@ -496,54 +374,90 @@
     <col customWidth="1" max="7" min="7" width="10.5"/>
     <col customWidth="1" max="8" min="8" width="11.5"/>
     <col customWidth="1" max="9" min="9" width="12.5"/>
-    <col customWidth="1" max="10" min="10" width="35.5"/>
+    <col customWidth="1" max="10" min="10" width="43.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>uid</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>links</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>derived</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>header</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>normative</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>reviewed</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s"/>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>1.2.3</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
+tempor incididunt ut labore et dolore magna aliqua.
+Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
+aliquip ex ea commodo consequat.
+Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
+eu fugiat nulla pariatur.
+Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
+deserunt mollit anim id est laborum.</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>SYS001
+SYS002:abc123</t>
+        </is>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>
@@ -551,27 +465,37 @@
       <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s"/>
+      <c r="H2" s="2" t="inlineStr"/>
       <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="2" t="s"/>
+      <c r="J2" s="2" t="inlineStr"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>REQ003</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>1.4</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Unicode: -40° ±1%</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>REF123</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
       </c>
       <c r="F3" s="2" t="b">
         <v>1</v>
@@ -579,77 +503,122 @@
       <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s"/>
+      <c r="H3" s="2" t="inlineStr"/>
       <c r="I3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s"/>
+      <c r="J3" s="2" t="inlineStr"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s"/>
-      <c r="E4" s="2" t="s"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>REQ004</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr"/>
+      <c r="E4" s="2" t="inlineStr"/>
       <c r="F4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s"/>
+      <c r="H4" s="2" t="inlineStr"/>
       <c r="I4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="2" t="s"/>
+      <c r="J4" s="2" t="inlineStr"/>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s"/>
-      <c r="E5" s="2" t="s"/>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>REQ002</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!
+```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
+@startuml
+Author --&gt; (Create Document)
+Author --&gt; (Create Item)
+Author --&gt; (Link Item to Document)
+Author --&gt; (Link Item to other Item)
+Author --&gt; (Edit Item)
+Author --&gt; (Review Item)
+Author -&gt; (Delete Item)
+Author -&gt; (Delete Document)
+(Export) &lt;- (Author)
+(Import) &lt;- (Author)
+Reviewer --&gt; (Review Item)
+System --&gt; (Suspect Changes)
+System --&gt; (Integrity)
+@enduml
+```</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr"/>
       <c r="F5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>Plantuml</t>
+        </is>
       </c>
       <c r="I5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>)ce6MY_!H_O8+v-th=&gt;p?J$&amp;#KhD7V1H+u;UNc)2</t>
+        </is>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s"/>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>REQ2-001</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!
+Test Math Expressions in Latex Style:
+Inline Style 1: $a \ne 0$
+Inline Style 2: \(ax^2 + bx + c = 0\)
+Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
       </c>
       <c r="F6" s="2" t="b">
         <v>1</v>
@@ -657,14 +626,14 @@
       <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="s"/>
+      <c r="H6" s="2" t="inlineStr"/>
       <c r="I6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="2" t="s"/>
+      <c r="J6" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update documentation links for the repository rename
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -1,137 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
-  </s:bookViews>
-  <s:sheets>
-    <s:sheet name="Sheet" sheetId="1" r:id="rId1"/>
-  </s:sheets>
-  <s:definedNames>
-    <s:definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</s:definedName>
-  </s:definedNames>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
-</s:workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
-  <si>
-    <t>uid</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>links</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>derived</t>
-  </si>
-  <si>
-    <t>header</t>
-  </si>
-  <si>
-    <t>normative</t>
-  </si>
-  <si>
-    <t>reviewed</t>
-  </si>
-  <si>
-    <t>REQ001</t>
-  </si>
-  <si>
-    <t>1.2.3</t>
-  </si>
-  <si>
-    <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
-tempor incididunt ut labore et dolore magna aliqua.
-Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
-aliquip ex ea commodo consequat.
-Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
-eu fugiat nulla pariatur.
-Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
-deserunt mollit anim id est laborum.</t>
-  </si>
-  <si>
-    <t>SYS001
-SYS002:abc123</t>
-  </si>
-  <si>
-    <t>REQ003</t>
-  </si>
-  <si>
-    <t>1.4</t>
-  </si>
-  <si>
-    <t>Unicode: -40° ±1%</t>
-  </si>
-  <si>
-    <t>REF123</t>
-  </si>
-  <si>
-    <t>REQ004</t>
-  </si>
-  <si>
-    <t>1.6</t>
-  </si>
-  <si>
-    <t>Hello, world!</t>
-  </si>
-  <si>
-    <t>REQ002</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>Hello, world!
-```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
-@startuml
-Author --&gt; (Create Document)
-Author --&gt; (Create Item)
-Author --&gt; (Link Item to Document)
-Author --&gt; (Link Item to other Item)
-Author --&gt; (Edit Item)
-Author --&gt; (Review Item)
-Author -&gt; (Delete Item)
-Author -&gt; (Delete Document)
-(Export) &lt;- (Author)
-(Import) &lt;- (Author)
-Reviewer --&gt; (Review Item)
-System --&gt; (Suspect Changes)
-System --&gt; (Integrity)
-@enduml
-```</t>
-  </si>
-  <si>
-    <t>Plantuml</t>
-  </si>
-  <si>
-    <t>50ae164a198e612dee696cc80942dc29</t>
-  </si>
-  <si>
-    <t>REQ2-001</t>
-  </si>
-  <si>
-    <t>Hello, world!
-Test Math Expressions in Latex Style:
-Inline Style 1: $a \ne 0$
-Inline Style 2: \(ax^2 + bx + c = 0\)
-Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
-  </si>
-</sst>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$J$1</definedName>
+  </definedNames>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -139,23 +21,19 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="00000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -174,18 +52,17 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
@@ -474,9 +351,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -485,7 +363,7 @@
       <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col customWidth="1" max="1" min="1" width="11.5"/>
     <col customWidth="1" max="2" min="2" width="8.5"/>
@@ -499,51 +377,87 @@
     <col customWidth="1" max="10" min="10" width="35.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>uid</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>level</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>ref</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>links</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>derived</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>header</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>normative</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>reviewed</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:10">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s"/>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>1.2.3</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Lorem ipsum dolor sit amet, consectetur adipiscing elit, sed do eiusmod
+tempor incididunt ut labore et dolore magna aliqua.
+Ut enim ad minim veniam, quis nostrud exercitation ullamco laboris nisi ut
+aliquip ex ea commodo consequat.
+Duis aute irure dolor in reprehenderit in voluptate velit esse cillum dolore
+eu fugiat nulla pariatur.
+Excepteur sint occaecat cupidatat non proident, sunt in culpa qui officia
+deserunt mollit anim id est laborum.</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr"/>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>SYS001
+SYS002:abc123</t>
+        </is>
       </c>
       <c r="F2" s="2" t="b">
         <v>1</v>
@@ -551,27 +465,37 @@
       <c r="G2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" s="2" t="s"/>
+      <c r="H2" s="2" t="inlineStr"/>
       <c r="I2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="2" t="s"/>
+      <c r="J2" s="2" t="inlineStr"/>
     </row>
-    <row r="3" spans="1:10">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>10</v>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>REQ003</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>1.4</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Unicode: -40° ±1%</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>REF123</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
       </c>
       <c r="F3" s="2" t="b">
         <v>1</v>
@@ -579,77 +503,122 @@
       <c r="G3" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H3" s="2" t="s"/>
+      <c r="H3" s="2" t="inlineStr"/>
       <c r="I3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="2" t="s"/>
+      <c r="J3" s="2" t="inlineStr"/>
     </row>
-    <row r="4" spans="1:10">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="2" t="s"/>
-      <c r="E4" s="2" t="s"/>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>REQ004</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>1.6</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr"/>
+      <c r="E4" s="2" t="inlineStr"/>
       <c r="F4" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G4" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="2" t="s"/>
+      <c r="H4" s="2" t="inlineStr"/>
       <c r="I4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="2" t="s"/>
+      <c r="J4" s="2" t="inlineStr"/>
     </row>
-    <row r="5" spans="1:10">
-      <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="2" t="s"/>
-      <c r="E5" s="2" t="s"/>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>REQ002</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!
+```plantuml format="svg_inline" alt="Use Cases of Doorstop" title="Use Cases of Doorstop"
+@startuml
+Author --&gt; (Create Document)
+Author --&gt; (Create Item)
+Author --&gt; (Link Item to Document)
+Author --&gt; (Link Item to other Item)
+Author --&gt; (Edit Item)
+Author --&gt; (Review Item)
+Author -&gt; (Delete Item)
+Author -&gt; (Delete Document)
+(Export) &lt;- (Author)
+(Import) &lt;- (Author)
+Reviewer --&gt; (Review Item)
+System --&gt; (Suspect Changes)
+System --&gt; (Integrity)
+@enduml
+```</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr"/>
       <c r="F5" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G5" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>24</v>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>Plantuml</t>
+        </is>
       </c>
       <c r="I5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="2" t="s">
-        <v>25</v>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>50ae164a198e612dee696cc80942dc29</t>
+        </is>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="A6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="2" t="s"/>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>REQ2-001</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>2.1</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Hello, world!
+Test Math Expressions in Latex Style:
+Inline Style 1: $a \ne 0$
+Inline Style 2: \(ax^2 + bx + c = 0\)
+Multiline: $$x = {-b \pm \sqrt{b^2-4ac} \over 2a}.$$</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>REQ001</t>
+        </is>
       </c>
       <c r="F6" s="2" t="b">
         <v>1</v>
@@ -657,14 +626,14 @@
       <c r="G6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="2" t="s"/>
+      <c r="H6" s="2" t="inlineStr"/>
       <c r="I6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="J6" s="2" t="s"/>
+      <c r="J6" s="2" t="inlineStr"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J1"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WIP: add 'keyword' to all of the remaining places in code
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -369,7 +369,7 @@
     <col customWidth="1" max="2" min="2" width="8.5"/>
     <col customWidth="1" max="3" min="3" width="65"/>
     <col customWidth="1" max="4" min="4" width="9.5"/>
-    <col customWidth="1" max="5" min="5" width="36.5"/>
+    <col customWidth="1" max="5" min="5" width="50.5"/>
     <col customWidth="1" max="6" min="6" width="42.5"/>
     <col customWidth="1" max="7" min="7" width="9.5"/>
     <col customWidth="1" max="8" min="8" width="10.5"/>
@@ -536,7 +536,7 @@
       <c r="D4" s="2" t="inlineStr"/>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>type:file,path:external/text.txt
+          <t>type:file,path:external/text.txt,keyword:REF123
 type:file,path:external/text2.txt</t>
         </is>
       </c>

</xml_diff>

<commit_message>
Update test files for Python 3.9
</commit_message>
<xml_diff>
--- a/doorstop/core/tests/files/exported.xlsx
+++ b/doorstop/core/tests/files/exported.xlsx
@@ -4,13 +4,13 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Sheet'!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sheet'!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -49,21 +49,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -359,23 +359,23 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="A1" pane="bottomLeft" sqref="A1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" width="11.5"/>
-    <col customWidth="1" max="2" min="2" width="8.5"/>
-    <col customWidth="1" max="3" min="3" width="65"/>
-    <col customWidth="1" max="4" min="4" width="9.5"/>
-    <col customWidth="1" max="5" min="5" width="50.5"/>
-    <col customWidth="1" max="6" min="6" width="42.5"/>
-    <col customWidth="1" max="7" min="7" width="9.5"/>
-    <col customWidth="1" max="8" min="8" width="10.5"/>
-    <col customWidth="1" max="9" min="9" width="11.5"/>
-    <col customWidth="1" max="10" min="10" width="12.5"/>
-    <col customWidth="1" max="11" min="11" width="47.5"/>
+    <col width="11.5" customWidth="1" min="1" max="1"/>
+    <col width="8.5" customWidth="1" min="2" max="2"/>
+    <col width="65" customWidth="1" min="3" max="3"/>
+    <col width="9.5" customWidth="1" min="4" max="4"/>
+    <col width="50.5" customWidth="1" min="5" max="5"/>
+    <col width="42.5" customWidth="1" min="6" max="6"/>
+    <col width="9.5" customWidth="1" min="7" max="7"/>
+    <col width="10.5" customWidth="1" min="8" max="8"/>
+    <col width="11.5" customWidth="1" min="9" max="9"/>
+    <col width="12.5" customWidth="1" min="10" max="10"/>
+    <col width="47.5" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -689,6 +689,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K1"/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>